<commit_message>
added Rac, Dext, kg
</commit_message>
<xml_diff>
--- a/Code/Results/res_bus/p_mw.xlsx
+++ b/Code/Results/res_bus/p_mw.xlsx
@@ -433,7 +433,7 @@
         <v>95.76379502855229</v>
       </c>
       <c r="G2">
-        <v>-218.1087349609977</v>
+        <v>-215.3074555466683</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -477,7 +477,7 @@
         <v>89.49015460996031</v>
       </c>
       <c r="G3">
-        <v>-202.5164348204743</v>
+        <v>-200.1541353621739</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -512,7 +512,7 @@
         <v>228.7231807617023</v>
       </c>
       <c r="D4">
-        <v>85.38998748436887</v>
+        <v>85.38998748436885</v>
       </c>
       <c r="E4">
         <v>85.38998748436882</v>
@@ -521,7 +521,7 @@
         <v>85.38998748436882</v>
       </c>
       <c r="G4">
-        <v>-192.4798232274284</v>
+        <v>-190.371676368487</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -556,7 +556,7 @@
         <v>224.0800688268934</v>
       </c>
       <c r="D5">
-        <v>83.65655902870685</v>
+        <v>83.65655902870688</v>
       </c>
       <c r="E5">
         <v>83.65655902870685</v>
@@ -565,7 +565,7 @@
         <v>83.65655902870685</v>
       </c>
       <c r="G5">
-        <v>-188.2702742258649</v>
+        <v>-186.2626070719929</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -609,7 +609,7 @@
         <v>83.36493964733984</v>
       </c>
       <c r="G6">
-        <v>-187.5639779839937</v>
+        <v>-185.5728286247045</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -653,7 +653,7 @@
         <v>85.36686348056003</v>
       </c>
       <c r="G7">
-        <v>-192.4235396560291</v>
+        <v>-190.3167594965325</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -697,7 +697,7 @@
         <v>93.6520320854782</v>
       </c>
       <c r="G8">
-        <v>-212.8265182842408</v>
+        <v>-210.1803155584764</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -732,16 +732,16 @@
         <v>289.1214906556616</v>
       </c>
       <c r="D9">
-        <v>107.9386898447803</v>
+        <v>107.9386898447804</v>
       </c>
       <c r="E9">
         <v>107.9386898447804</v>
       </c>
       <c r="F9">
-        <v>107.9386898447804</v>
+        <v>107.9386898447803</v>
       </c>
       <c r="G9">
-        <v>-249.3401160954811</v>
+        <v>-245.46707268136</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -785,7 +785,7 @@
         <v>117.2512402288745</v>
       </c>
       <c r="G10">
-        <v>-274.3608153773955</v>
+        <v>-269.3873981896476</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -814,22 +814,22 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>-432.9753410696504</v>
+        <v>-432.9753410696505</v>
       </c>
       <c r="C11">
-        <v>324.7315058022378</v>
+        <v>324.7315058022379</v>
       </c>
       <c r="D11">
+        <v>121.2330954995022</v>
+      </c>
+      <c r="E11">
         <v>121.2330954995021</v>
-      </c>
-      <c r="E11">
-        <v>121.2330954995022</v>
       </c>
       <c r="F11">
         <v>121.2330954995022</v>
       </c>
       <c r="G11">
-        <v>-285.4614995291461</v>
+        <v>-279.9073060755944</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -873,7 +873,7 @@
         <v>122.7045135760076</v>
       </c>
       <c r="G12">
-        <v>-289.638679811275</v>
+        <v>-283.8477475878325</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -902,10 +902,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-437.1044095295264</v>
+        <v>-437.1044095295265</v>
       </c>
       <c r="C13">
-        <v>327.8283071471448</v>
+        <v>327.8283071471449</v>
       </c>
       <c r="D13">
         <v>122.3892346682674</v>
@@ -914,10 +914,10 @@
         <v>122.3892346682674</v>
       </c>
       <c r="F13">
-        <v>122.3892346682674</v>
+        <v>122.3892346682675</v>
       </c>
       <c r="G13">
-        <v>-288.7399321712532</v>
+        <v>-283.0008498503894</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -961,7 +961,7 @@
         <v>121.3548789831807</v>
       </c>
       <c r="G14">
-        <v>-285.8055853548794</v>
+        <v>-280.232292859933</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -999,13 +999,13 @@
         <v>120.7165677442802</v>
       </c>
       <c r="E15">
+        <v>120.7165677442803</v>
+      </c>
+      <c r="F15">
         <v>120.7165677442802</v>
       </c>
-      <c r="F15">
-        <v>120.7165677442803</v>
-      </c>
       <c r="G15">
-        <v>-284.0052942792691</v>
+        <v>-278.5311582840544</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1034,13 +1034,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-417.8068230501004</v>
+        <v>-417.8068230501005</v>
       </c>
       <c r="C16">
-        <v>313.3551172875753</v>
+        <v>313.3551172875754</v>
       </c>
       <c r="D16">
-        <v>116.9859104540281</v>
+        <v>116.9859104540282</v>
       </c>
       <c r="E16">
         <v>116.9859104540282</v>
@@ -1049,7 +1049,7 @@
         <v>116.9859104540282</v>
       </c>
       <c r="G16">
-        <v>-273.6307713626062</v>
+        <v>-268.6933036005295</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1078,7 +1078,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>-409.4007760748645</v>
+        <v>-409.4007760748646</v>
       </c>
       <c r="C17">
         <v>307.0505820561484</v>
@@ -1087,13 +1087,13 @@
         <v>114.6322173009621</v>
       </c>
       <c r="E17">
-        <v>114.632217300962</v>
+        <v>114.6322173009621</v>
       </c>
       <c r="F17">
         <v>114.6322173009621</v>
       </c>
       <c r="G17">
-        <v>-267.2026066954416</v>
+        <v>-262.5708380849388</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>-404.4802617114975</v>
       </c>
       <c r="C18">
-        <v>303.3601962836232</v>
+        <v>303.3601962836231</v>
       </c>
       <c r="D18">
         <v>113.2544732792193</v>
@@ -1137,7 +1137,7 @@
         <v>113.2544732792193</v>
       </c>
       <c r="G18">
-        <v>-263.4777276913297</v>
+        <v>-259.0146630298199</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1181,7 +1181,7 @@
         <v>112.7838721813715</v>
       </c>
       <c r="G19">
-        <v>-262.2114715170633</v>
+        <v>-257.8044238579542</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>114.8852507032591</v>
       </c>
       <c r="G20">
-        <v>-267.8896650536754</v>
+        <v>-263.2261217359288</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1254,22 +1254,22 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>-434.4988625867514</v>
+        <v>-434.4988625867515</v>
       </c>
       <c r="C21">
-        <v>325.8741469400636</v>
+        <v>325.8741469400637</v>
       </c>
       <c r="D21">
         <v>121.6596815242904</v>
       </c>
       <c r="E21">
-        <v>121.6596815242904</v>
+        <v>121.6596815242905</v>
       </c>
       <c r="F21">
         <v>121.6596815242904</v>
       </c>
       <c r="G21">
-        <v>-286.6680480823499</v>
+        <v>-281.0465719734139</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -1313,7 +1313,7 @@
         <v>125.8749334216475</v>
       </c>
       <c r="G22">
-        <v>-298.7987040630508</v>
+        <v>-292.4481453277631</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1342,7 +1342,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>-441.5876354132126</v>
+        <v>-441.5876354132125</v>
       </c>
       <c r="C23">
         <v>331.1907265599094</v>
@@ -1357,7 +1357,7 @@
         <v>123.6445379156995</v>
       </c>
       <c r="G23">
-        <v>-292.3308759600409</v>
+        <v>-286.3814958821378</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1401,7 +1401,7 @@
         <v>114.7709308588577</v>
       </c>
       <c r="G24">
-        <v>-267.5791380168116</v>
+        <v>-262.9299816402682</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>104.2824822117912</v>
       </c>
       <c r="G25">
-        <v>-239.8081646574913</v>
+        <v>-236.2929982387788</v>
       </c>
       <c r="H25">
         <v>0</v>

</xml_diff>